<commit_message>
added share allocation, installed capacity and ramp info
</commit_message>
<xml_diff>
--- a/dbHelpers/generator_info.xlsx
+++ b/dbHelpers/generator_info.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20346"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nagasudhir\Documents\NodeJS Projects\ine_info_node_webhook\dbHelpers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POSOCO\IT\NodeJS Projects\ine_info_node_webhook\dbHelpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7FC4555-27D8-428C-A4E7-4F5EA2078AA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>name</t>
   </si>
@@ -42,12 +43,69 @@
   </si>
   <si>
     <t>Gadarwara</t>
+  </si>
+  <si>
+    <t>VSTPS_Stage_1</t>
+  </si>
+  <si>
+    <t>Solapur</t>
+  </si>
+  <si>
+    <t>CGPL</t>
+  </si>
+  <si>
+    <t>Mouda</t>
+  </si>
+  <si>
+    <t>Mouda_Stage_2</t>
+  </si>
+  <si>
+    <t>Sasan</t>
+  </si>
+  <si>
+    <t>NSPCL</t>
+  </si>
+  <si>
+    <t>Gandhar</t>
+  </si>
+  <si>
+    <t>Kawas</t>
+  </si>
+  <si>
+    <t>Sipat_Stage_1</t>
+  </si>
+  <si>
+    <t>Sipat_Stage_2</t>
+  </si>
+  <si>
+    <t>VSTPS_Stage_2</t>
+  </si>
+  <si>
+    <t>VSTPS_Stage_3</t>
+  </si>
+  <si>
+    <t>VSTPS_Stage_4</t>
+  </si>
+  <si>
+    <t>VSTPS_Stage_5</t>
+  </si>
+  <si>
+    <t>KSTPS_Stage_1</t>
+  </si>
+  <si>
+    <t>KSTPS_Stage_2</t>
+  </si>
+  <si>
+    <t>KSTPS_Stage_3</t>
+  </si>
+  <si>
+    <t>RGPPL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -77,9 +135,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -361,16 +422,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
@@ -398,17 +459,340 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>800</v>
       </c>
       <c r="C2">
         <v>1600</v>
       </c>
       <c r="D2">
-        <v>237</v>
+        <v>201</v>
       </c>
       <c r="E2">
-        <v>377</v>
+        <v>373</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1320</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1320</v>
+      </c>
+      <c r="D3">
+        <v>174</v>
+      </c>
+      <c r="E3">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4150</v>
+      </c>
+      <c r="C4" s="2">
+        <v>4150</v>
+      </c>
+      <c r="D4">
+        <v>902</v>
+      </c>
+      <c r="E4">
+        <v>1951</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D5">
+        <v>190</v>
+      </c>
+      <c r="E5">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1320</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1320</v>
+      </c>
+      <c r="D6">
+        <v>150</v>
+      </c>
+      <c r="E6">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3960</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3960</v>
+      </c>
+      <c r="D7">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="2">
+        <v>500</v>
+      </c>
+      <c r="C8" s="2">
+        <v>500</v>
+      </c>
+      <c r="D8">
+        <v>172</v>
+      </c>
+      <c r="E8">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="2">
+        <v>687.90000000000009</v>
+      </c>
+      <c r="C9" s="2">
+        <v>687.90000000000009</v>
+      </c>
+      <c r="D9">
+        <v>108</v>
+      </c>
+      <c r="E9">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="2">
+        <v>656.2</v>
+      </c>
+      <c r="C10" s="2">
+        <v>656.2</v>
+      </c>
+      <c r="D10">
+        <v>85</v>
+      </c>
+      <c r="E10">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1980</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1980</v>
+      </c>
+      <c r="D11">
+        <v>132</v>
+      </c>
+      <c r="E11">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D12">
+        <v>125</v>
+      </c>
+      <c r="E12">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1260</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1260</v>
+      </c>
+      <c r="D13">
+        <v>86</v>
+      </c>
+      <c r="E13">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D14">
+        <v>71</v>
+      </c>
+      <c r="E14">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D15">
+        <v>105</v>
+      </c>
+      <c r="E15">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1000</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D16">
+        <v>158</v>
+      </c>
+      <c r="E16">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2">
+        <v>500</v>
+      </c>
+      <c r="C17" s="2">
+        <v>500</v>
+      </c>
+      <c r="D17">
+        <v>169</v>
+      </c>
+      <c r="E17">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2">
+        <v>600</v>
+      </c>
+      <c r="C18" s="2">
+        <v>600</v>
+      </c>
+      <c r="D18">
+        <v>69</v>
+      </c>
+      <c r="E18">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1500</v>
+      </c>
+      <c r="C19" s="2">
+        <v>1500</v>
+      </c>
+      <c r="D19">
+        <v>69</v>
+      </c>
+      <c r="E19">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2">
+        <v>500</v>
+      </c>
+      <c r="C20" s="2">
+        <v>500</v>
+      </c>
+      <c r="D20">
+        <v>140</v>
+      </c>
+      <c r="E20">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1967</v>
+      </c>
+      <c r="C21" s="2">
+        <v>1967</v>
+      </c>
+      <c r="D21">
+        <v>130</v>
+      </c>
+      <c r="E21">
+        <v>368</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lara ultimate cap updated
</commit_message>
<xml_diff>
--- a/dbHelpers/generator_info.xlsx
+++ b/dbHelpers/generator_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POSOCO\IT\NodeJS Projects\ine_info_node_webhook\dbHelpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F6435C-FC65-4A3D-B628-524CD64DBAAF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD54838C-DDBB-4BE4-BA31-F3050E8D39B3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -498,7 +498,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1266,7 +1266,7 @@
         <v>800</v>
       </c>
       <c r="C45" s="1">
-        <v>800</v>
+        <v>1600</v>
       </c>
       <c r="D45">
         <v>199</v>

</xml_diff>